<commit_message>
fix:  change target mail to referent when group of visitors
</commit_message>
<xml_diff>
--- a/tests/helpers/xlsxFile.xlsx
+++ b/tests/helpers/xlsxFile.xlsx
@@ -20,62 +20,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">MINARM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NID*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type d'employé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prénom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom de Naissance</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">MINARM*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type d'employé*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prénom*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom de Naissance*</t>
   </si>
   <si>
     <t xml:space="preserve">Nom d'usage</t>
   </si>
   <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grade*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unité / Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIP</t>
+    <t xml:space="preserve">Grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unité / Entreprise*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIP*</t>
   </si>
   <si>
     <t xml:space="preserve">Motif VIP</t>
   </si>
   <si>
-    <t xml:space="preserve">Nationalité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de Naissance [jj/mm/aaaa]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu de Naissance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type document identité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numéro document identité</t>
+    <t xml:space="preserve">Nationalité*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date de Naissance [jj/mm/aaaa]*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu de Naissance*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type document identité*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro document identité*</t>
   </si>
   <si>
     <t xml:space="preserve">oui</t>
   </si>
   <si>
-    <t xml:space="preserve">Nid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visiteur</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email@localhost</t>
   </si>
   <si>
     <t xml:space="preserve">Unity</t>
@@ -211,13 +202,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.32"/>
@@ -225,16 +216,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="51.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="51.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,96 +273,87 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="0" t="n">
+      <c r="O2" s="0" t="n">
         <v>4567</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="N3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>123456789</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>